<commit_message>
Fixed MultiProducersMultiConsumersUnlimitedLockFreeQueue_v5 - all tests passing
</commit_message>
<xml_diff>
--- a/doc/MPMC_queue.xlsx
+++ b/doc/MPMC_queue.xlsx
@@ -11,16 +11,62 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+  <si>
+    <t>Algo:</t>
+  </si>
+  <si>
+    <t>MultiProducersMultiConsumersUnlimitedLockFreeQueue_v4</t>
+  </si>
+  <si>
+    <t>size = 0</t>
+  </si>
+  <si>
+    <t>first_a = nullptr, last_a = nullptr</t>
+  </si>
+  <si>
+    <t>size = 1</t>
+  </si>
+  <si>
+    <t>first_a = last_a</t>
+  </si>
+  <si>
+    <t>case 1</t>
+  </si>
+  <si>
+    <t>case 2</t>
+  </si>
+  <si>
+    <t>pop()</t>
+  </si>
+  <si>
+    <t>push()</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -46,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,13 +389,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="3" max="3" width="73.5703125" customWidth="1"/>
+    <col min="4" max="4" width="54.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>